<commit_message>
Adding NIR data and metadata
</commit_message>
<xml_diff>
--- a/studies/September 2023 - Western Cape Breton/data/metadata.xlsx
+++ b/studies/September 2023 - Western Cape Breton/data/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SuretteTJ\Desktop\github\snow-crab-measurement-project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SuretteTJ\Desktop\github\snow-crab-measurement-project\studies\September 2023 - Western Cape Breton\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B837C3-EFB9-4E08-9CF9-57417D2DF402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13689632-D4DC-47B2-96CC-D9F3190EDEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="465" windowWidth="26880" windowHeight="14880" xr2:uid="{15E8C65C-F855-4515-85F9-BEE2D7C191F8}"/>
+    <workbookView xWindow="-28230" yWindow="1710" windowWidth="26460" windowHeight="11580" activeTab="1" xr2:uid="{15E8C65C-F855-4515-85F9-BEE2D7C191F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="93">
   <si>
     <t>date</t>
   </si>
@@ -139,9 +139,6 @@
     <t>hemolymph</t>
   </si>
   <si>
-    <t>Crab chela durometer reading (1-100).</t>
-  </si>
-  <si>
     <t>durometer</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>longitude</t>
   </si>
   <si>
-    <t>Name of sampler(s).</t>
-  </si>
-  <si>
     <t>sampler</t>
   </si>
   <si>
@@ -290,6 +284,39 @@
   </si>
   <si>
     <t>Snow crab NIR data from September 2023 study.</t>
+  </si>
+  <si>
+    <t>The device aperture requires that a protective film be applied during sampling.</t>
+  </si>
+  <si>
+    <t>There will be two types of sampling gear : the survey Neprops trawl or commercial conical traps.</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>trawl; trap</t>
+  </si>
+  <si>
+    <t>m; f</t>
+  </si>
+  <si>
+    <t>Crab chela durometer reading.</t>
+  </si>
+  <si>
+    <t>1-100</t>
+  </si>
+  <si>
+    <t>Name(s) of sampler(s).</t>
+  </si>
+  <si>
+    <t>sample.id</t>
+  </si>
+  <si>
+    <t>Sample identification.</t>
+  </si>
+  <si>
+    <t>pastic disk; SaranWrap; cellular protective film</t>
   </si>
 </sst>
 </file>
@@ -661,44 +688,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544A1CC2-C373-43FA-B861-C2AAC9D5F0EE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="92.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="92.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -709,249 +738,283 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD43587-0DB0-4157-834F-7F7B11770A21}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43" customWidth="1"/>
+    <col min="4" max="4" width="85.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>11</v>
       </c>
     </row>
@@ -969,100 +1032,100 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="101.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="101.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>